<commit_message>
컬럼 변경 (lecture- content 삭제, lecture_detail - introduce, curriculum 추가) 그에 따른 DML 수정 + lecture_category 8개 확정
</commit_message>
<xml_diff>
--- a/테이블.xlsx
+++ b/테이블.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="20730" windowHeight="11760"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="156">
   <si>
     <t>컬럼 명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar2()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>not null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -130,10 +126,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>varchar2()</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -620,6 +612,22 @@
   </si>
   <si>
     <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>freeBoard_title(게시글 제목)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar2(300)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1351,7 +1359,7 @@
   <dimension ref="A1:R140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1379,7 +1387,7 @@
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="38"/>
@@ -1388,7 +1396,7 @@
       </c>
       <c r="I1" s="33"/>
       <c r="J1" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K1" s="37"/>
       <c r="L1" s="38"/>
@@ -1419,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>0</v>
@@ -1434,15 +1442,15 @@
         <v>4</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -1450,142 +1458,142 @@
       <c r="D4" s="1"/>
       <c r="E4" s="3"/>
       <c r="H4" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" s="11"/>
       <c r="H5" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3"/>
       <c r="H6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K6" s="24"/>
       <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="3"/>
       <c r="H7" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K7" s="24"/>
       <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K8" s="24"/>
       <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
       <c r="H9" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -1593,21 +1601,21 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
       <c r="H10" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
@@ -1615,13 +1623,13 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="3"/>
@@ -1633,13 +1641,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="3"/>
@@ -1651,10 +1659,10 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1780,7 +1788,7 @@
       </c>
       <c r="B27" s="33"/>
       <c r="C27" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="38"/>
@@ -1789,7 +1797,7 @@
       </c>
       <c r="I27" s="33"/>
       <c r="J27" s="36" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K27" s="37"/>
       <c r="L27" s="38"/>
@@ -1798,7 +1806,7 @@
       </c>
       <c r="O27" s="33"/>
       <c r="P27" s="36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q27" s="37"/>
       <c r="R27" s="38"/>
@@ -1834,7 +1842,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" s="7" t="s">
         <v>0</v>
@@ -1849,7 +1857,7 @@
         <v>4</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N29" s="7" t="s">
         <v>0</v>
@@ -1864,15 +1872,15 @@
         <v>4</v>
       </c>
       <c r="R29" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
@@ -1880,10 +1888,10 @@
       <c r="D30" s="1"/>
       <c r="E30" s="3"/>
       <c r="H30" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>3</v>
@@ -1891,10 +1899,10 @@
       <c r="K30" s="1"/>
       <c r="L30" s="3"/>
       <c r="N30" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>3</v>
@@ -1904,141 +1912,143 @@
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E31" s="3"/>
       <c r="H31" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L31" s="3"/>
       <c r="N31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O31" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R31" s="3"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E32" s="25"/>
       <c r="H32" s="2" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="3"/>
       <c r="N32" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q32" s="1"/>
       <c r="R32" s="3"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D33" s="24"/>
       <c r="E33" s="25"/>
       <c r="H33" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J33" s="1"/>
+        <v>129</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="K33" s="1"/>
       <c r="L33" s="3"/>
       <c r="N33" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q33" s="1"/>
       <c r="R33" s="3"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D34" s="24"/>
       <c r="E34" s="25"/>
       <c r="H34" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="3"/>
       <c r="N34" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
@@ -2046,32 +2056,30 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="24"/>
       <c r="E35" s="25"/>
       <c r="H35" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
-      <c r="L35" s="3">
-        <v>0</v>
-      </c>
+      <c r="L35" s="3"/>
       <c r="N35" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -2079,32 +2087,32 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D36" s="24"/>
       <c r="E36" s="25"/>
       <c r="H36" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="3" t="s">
-        <v>30</v>
+      <c r="L36" s="3">
+        <v>0</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2114,44 +2122,50 @@
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D37" s="24"/>
       <c r="E37" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="3"/>
+      <c r="L37" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="N37" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:18">
       <c r="A38" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C38" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D38" s="24"/>
       <c r="E38" s="25"/>
@@ -2168,13 +2182,13 @@
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="25"/>
@@ -2191,13 +2205,13 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D40" s="24"/>
       <c r="E40" s="25"/>
@@ -2214,13 +2228,13 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D41" s="24"/>
       <c r="E41" s="25"/>
@@ -2237,10 +2251,10 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
@@ -2369,7 +2383,7 @@
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D53" s="37"/>
       <c r="E53" s="38"/>
@@ -2378,7 +2392,7 @@
       </c>
       <c r="I53" s="33"/>
       <c r="J53" s="36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K53" s="37"/>
       <c r="L53" s="38"/>
@@ -2387,7 +2401,7 @@
       </c>
       <c r="O53" s="33"/>
       <c r="P53" s="36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="Q53" s="37"/>
       <c r="R53" s="38"/>
@@ -2423,7 +2437,7 @@
         <v>4</v>
       </c>
       <c r="E55" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H55" s="7" t="s">
         <v>0</v>
@@ -2438,7 +2452,7 @@
         <v>4</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N55" s="7" t="s">
         <v>0</v>
@@ -2453,28 +2467,28 @@
         <v>4</v>
       </c>
       <c r="R55" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B56" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E56" s="3"/>
       <c r="H56" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J56" s="1" t="s">
         <v>3</v>
@@ -2482,10 +2496,10 @@
       <c r="K56" s="1"/>
       <c r="L56" s="3"/>
       <c r="N56" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P56" s="1" t="s">
         <v>3</v>
@@ -2495,162 +2509,162 @@
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E57" s="3"/>
       <c r="H57" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="O57" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="R57" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
       <c r="E58" s="25"/>
       <c r="H58" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L58" s="3"/>
       <c r="N58" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O58" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R58" s="3"/>
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
       <c r="E59" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K59" s="1"/>
       <c r="L59" s="3"/>
       <c r="N59" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P59" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q59" s="1"/>
       <c r="R59" s="3"/>
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C60" s="24"/>
       <c r="D60" s="24"/>
       <c r="E60" s="25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K60" s="1"/>
       <c r="L60" s="3"/>
       <c r="N60" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q60" s="1"/>
       <c r="R60" s="3"/>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C61" s="16"/>
       <c r="D61" s="16"/>
@@ -2668,10 +2682,10 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16"/>
@@ -2689,10 +2703,10 @@
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -2868,7 +2882,7 @@
       </c>
       <c r="B77" s="33"/>
       <c r="C77" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D77" s="37"/>
       <c r="E77" s="38"/>
@@ -2877,7 +2891,7 @@
       </c>
       <c r="I77" s="33"/>
       <c r="J77" s="36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K77" s="37"/>
       <c r="L77" s="38"/>
@@ -2908,7 +2922,7 @@
         <v>4</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H79" s="27" t="s">
         <v>0</v>
@@ -2923,15 +2937,15 @@
         <v>4</v>
       </c>
       <c r="L79" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:18">
       <c r="A80" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>3</v>
@@ -2939,42 +2953,44 @@
       <c r="D80" s="1"/>
       <c r="E80" s="3"/>
       <c r="H80" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I80" s="21" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="J80" s="21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K80" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L80" s="31"/>
+        <v>29</v>
+      </c>
+      <c r="L80" s="31" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="3"/>
       <c r="H81" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L81" s="3"/>
     </row>
@@ -2985,16 +3001,16 @@
       <c r="D82" s="1"/>
       <c r="E82" s="3"/>
       <c r="H82" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>6</v>
+        <v>122</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L82" s="3"/>
     </row>
@@ -3173,7 +3189,7 @@
       </c>
       <c r="B99" s="33"/>
       <c r="C99" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D99" s="37"/>
       <c r="E99" s="38"/>
@@ -3182,7 +3198,7 @@
       </c>
       <c r="I99" s="33"/>
       <c r="J99" s="36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K99" s="37"/>
       <c r="L99" s="38"/>
@@ -3213,7 +3229,7 @@
         <v>4</v>
       </c>
       <c r="E101" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H101" s="7" t="s">
         <v>0</v>
@@ -3228,147 +3244,153 @@
         <v>4</v>
       </c>
       <c r="L101" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C102" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D102" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E102" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L102" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C103" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D103" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E103" s="25"/>
       <c r="H103" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L103" s="3"/>
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B104" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C104" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D104" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E104" s="25"/>
       <c r="H104" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L104" s="3"/>
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B105" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C105" s="24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D105" s="24"/>
       <c r="E105" s="25"/>
       <c r="H105" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K105" s="1"/>
       <c r="L105" s="3"/>
     </row>
     <row r="106" spans="1:12">
       <c r="A106" s="23" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B106" s="24" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="C106" s="24" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D106" s="24"/>
       <c r="E106" s="25"/>
       <c r="H106" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="L106" s="3"/>
     </row>
     <row r="107" spans="1:12">
-      <c r="A107" s="23"/>
-      <c r="B107" s="24"/>
-      <c r="C107" s="24"/>
+      <c r="A107" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B107" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="24" t="s">
+        <v>6</v>
+      </c>
       <c r="D107" s="24"/>
       <c r="E107" s="25"/>
       <c r="H107" s="2"/>
@@ -3513,7 +3535,7 @@
       </c>
       <c r="B121" s="33"/>
       <c r="C121" s="36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D121" s="37"/>
       <c r="E121" s="38"/>
@@ -3539,32 +3561,40 @@
         <v>4</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124" spans="1:12">
       <c r="A124" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B124" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
-      <c r="E124" s="3"/>
+      <c r="E124" s="3" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="125" spans="1:12">
       <c r="A125" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B125" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:12">
       <c r="A126" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B126" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="3"/>
@@ -3669,6 +3699,20 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A99:B100"/>
+    <mergeCell ref="C99:E100"/>
+    <mergeCell ref="H99:I100"/>
+    <mergeCell ref="J99:L100"/>
+    <mergeCell ref="A121:B122"/>
+    <mergeCell ref="C121:E122"/>
+    <mergeCell ref="C77:E78"/>
+    <mergeCell ref="J77:L78"/>
+    <mergeCell ref="A53:B54"/>
+    <mergeCell ref="H53:I54"/>
+    <mergeCell ref="A77:B78"/>
+    <mergeCell ref="H77:I78"/>
+    <mergeCell ref="J53:L54"/>
+    <mergeCell ref="C53:E54"/>
     <mergeCell ref="N27:O28"/>
     <mergeCell ref="P27:R28"/>
     <mergeCell ref="N53:O54"/>
@@ -3681,20 +3725,6 @@
     <mergeCell ref="J1:L2"/>
     <mergeCell ref="C27:E28"/>
     <mergeCell ref="J27:L28"/>
-    <mergeCell ref="C77:E78"/>
-    <mergeCell ref="J77:L78"/>
-    <mergeCell ref="A53:B54"/>
-    <mergeCell ref="H53:I54"/>
-    <mergeCell ref="A77:B78"/>
-    <mergeCell ref="H77:I78"/>
-    <mergeCell ref="J53:L54"/>
-    <mergeCell ref="C53:E54"/>
-    <mergeCell ref="A99:B100"/>
-    <mergeCell ref="C99:E100"/>
-    <mergeCell ref="H99:I100"/>
-    <mergeCell ref="J99:L100"/>
-    <mergeCell ref="A121:B122"/>
-    <mergeCell ref="C121:E122"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>